<commit_message>
Carga preinscrito BD FULL
</commit_message>
<xml_diff>
--- a/BACKEND/aantik/preinscritos.xlsx
+++ b/BACKEND/aantik/preinscritos.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUCHYS\Documents\workspace-spring-tool-suite-4-4.11.0.RELEASE\aantik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUCHYS\Documents\GitHub\AANTIK\BACKEND\aantik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6522CD79-565C-42CB-BF54-C59898430E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F1081D-0725-4FE7-8EBA-4B319178A57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1786,7 +1797,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1829,18 +1843,19 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J158" totalsRowShown="0">
-  <autoFilter ref="A1:J158" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Nombre completo " dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DE124EEB-5A38-4D4B-8F5F-B30C38CF7814}" name="Correo institucional"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ID de la Javeriana incluyendo los ceros y sin puntos" dataDxfId="6"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Cédula de ciudadanía (sin puntos ó comas)" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Materia a matricular en 2022-30" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="¿Asististe en semestres anteriores al Taller Sentido Mi Práctica?" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Si la respuesta en la pregunta 5 es SI, por favor diligencia la fecha de asistencia. En caso negativo dejar en blanco" dataDxfId="2"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Por favor escribe tu número celular o en su defecto un teléfono de contacto" dataDxfId="1"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="¿Ya revisaste la infografía enviada por medio de correo de carrera y/o de correo de coordinaciónpgpt dónde se exponen los pasos a seguir para el registro de CDIO 3 ó PSU? En caso negativo te invit…" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Nombre completo " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DE124EEB-5A38-4D4B-8F5F-B30C38CF7814}" name="Correo institucional" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ID de la Javeriana incluyendo los ceros y sin puntos" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Cédula de ciudadanía (sin puntos ó comas)" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Materia a matricular en 2022-30" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="¿Asististe en semestres anteriores al Taller Sentido Mi Práctica?" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Si la respuesta en la pregunta 5 es SI, por favor diligencia la fecha de asistencia. En caso negativo dejar en blanco" dataDxfId="3"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Por favor escribe tu número celular o en su defecto un teléfono de contacto" dataDxfId="2"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="¿Ya revisaste la infografía enviada por medio de correo de carrera y/o de correo de coordinaciónpgpt dónde se exponen los pasos a seguir para el registro de CDIO 3 ó PSU? En caso negativo te invit…" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2145,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2198,6 +2213,10 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="2" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Luisa@prueba.com</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
@@ -2224,6 +2243,10 @@
       <c r="B3" t="s">
         <v>15</v>
       </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Isabe@prueba.com</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2250,6 +2273,10 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
+      <c r="C4" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Valer@prueba.com</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
@@ -2276,6 +2303,10 @@
       <c r="B5" t="s">
         <v>23</v>
       </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Valer@prueba.com</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
@@ -2302,6 +2333,10 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
+      <c r="C6" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sara @prueba.com</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
@@ -2328,6 +2363,10 @@
       <c r="B7" t="s">
         <v>32</v>
       </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Linda@prueba.com</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>33</v>
       </c>
@@ -2354,6 +2393,10 @@
       <c r="B8" t="s">
         <v>36</v>
       </c>
+      <c r="C8" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Luis @prueba.com</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
@@ -2383,6 +2426,10 @@
       <c r="B9" t="s">
         <v>42</v>
       </c>
+      <c r="C9" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jose @prueba.com</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>43</v>
       </c>
@@ -2412,6 +2459,10 @@
       <c r="B10" t="s">
         <v>47</v>
       </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Gabri@prueba.com</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>48</v>
       </c>
@@ -2438,6 +2489,10 @@
       <c r="B11" t="s">
         <v>51</v>
       </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Lina @prueba.com</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>52</v>
       </c>
@@ -2464,6 +2519,10 @@
       <c r="B12" t="s">
         <v>55</v>
       </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>nicol@prueba.com</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>56</v>
       </c>
@@ -2489,6 +2548,10 @@
       </c>
       <c r="B13" t="s">
         <v>59</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Esteb@prueba.com</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>60</v>
@@ -2516,6 +2579,10 @@
       <c r="B14" t="s">
         <v>63</v>
       </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>64</v>
       </c>
@@ -2541,6 +2608,10 @@
       </c>
       <c r="B15" t="s">
         <v>67</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Andre@prueba.com</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>68</v>
@@ -2568,6 +2639,10 @@
       <c r="B16" t="s">
         <v>71</v>
       </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maira@prueba.com</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>72</v>
       </c>
@@ -2594,6 +2669,10 @@
       <c r="B17" t="s">
         <v>75</v>
       </c>
+      <c r="C17" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>ANGEL@prueba.com</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>76</v>
       </c>
@@ -2620,6 +2699,10 @@
       <c r="B18" t="s">
         <v>79</v>
       </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Ximen@prueba.com</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>80</v>
       </c>
@@ -2646,6 +2729,10 @@
       <c r="B19" t="s">
         <v>83</v>
       </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>84</v>
       </c>
@@ -2672,6 +2759,10 @@
       <c r="B20" t="s">
         <v>87</v>
       </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>88</v>
       </c>
@@ -2698,6 +2789,10 @@
       <c r="B21" t="s">
         <v>91</v>
       </c>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Duvan@prueba.com</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>92</v>
       </c>
@@ -2724,6 +2819,10 @@
       <c r="B22" t="s">
         <v>95</v>
       </c>
+      <c r="C22" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Natal@prueba.com</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>96</v>
       </c>
@@ -2750,6 +2849,10 @@
       <c r="B23" t="s">
         <v>99</v>
       </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sergi@prueba.com</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>100</v>
       </c>
@@ -2776,6 +2879,10 @@
       <c r="B24" t="s">
         <v>103</v>
       </c>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>104</v>
       </c>
@@ -2802,6 +2909,10 @@
       <c r="B25" t="s">
         <v>107</v>
       </c>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D25" s="1" t="s">
         <v>108</v>
       </c>
@@ -2828,6 +2939,10 @@
       <c r="B26" t="s">
         <v>111</v>
       </c>
+      <c r="C26" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Tábat@prueba.com</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>112</v>
       </c>
@@ -2854,6 +2969,10 @@
       <c r="B27" t="s">
         <v>115</v>
       </c>
+      <c r="C27" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jorge@prueba.com</v>
+      </c>
       <c r="D27" s="1" t="s">
         <v>116</v>
       </c>
@@ -2880,6 +2999,10 @@
       <c r="B28" t="s">
         <v>119</v>
       </c>
+      <c r="C28" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Julia@prueba.com</v>
+      </c>
       <c r="D28" s="1" t="s">
         <v>120</v>
       </c>
@@ -2906,6 +3029,10 @@
       <c r="B29" t="s">
         <v>75</v>
       </c>
+      <c r="C29" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>ANGEL@prueba.com</v>
+      </c>
       <c r="D29" s="1" t="s">
         <v>76</v>
       </c>
@@ -2932,6 +3059,10 @@
       <c r="B30" t="s">
         <v>123</v>
       </c>
+      <c r="C30" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Aleja@prueba.com</v>
+      </c>
       <c r="D30" s="1" t="s">
         <v>124</v>
       </c>
@@ -2958,6 +3089,10 @@
       <c r="B31" t="s">
         <v>127</v>
       </c>
+      <c r="C31" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juani@prueba.com</v>
+      </c>
       <c r="D31" s="1" t="s">
         <v>128</v>
       </c>
@@ -2984,6 +3119,10 @@
       <c r="B32" t="s">
         <v>131</v>
       </c>
+      <c r="C32" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Catal@prueba.com</v>
+      </c>
       <c r="D32" s="1" t="s">
         <v>132</v>
       </c>
@@ -3010,6 +3149,10 @@
       <c r="B33" t="s">
         <v>135</v>
       </c>
+      <c r="C33" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D33" s="1" t="s">
         <v>136</v>
       </c>
@@ -3036,6 +3179,10 @@
       <c r="B34" t="s">
         <v>139</v>
       </c>
+      <c r="C34" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>André@prueba.com</v>
+      </c>
       <c r="D34" s="1" t="s">
         <v>140</v>
       </c>
@@ -3062,6 +3209,10 @@
       <c r="B35" t="s">
         <v>143</v>
       </c>
+      <c r="C35" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Julia@prueba.com</v>
+      </c>
       <c r="D35" s="1" t="s">
         <v>144</v>
       </c>
@@ -3088,6 +3239,10 @@
       <c r="B36" t="s">
         <v>147</v>
       </c>
+      <c r="C36" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D36" s="1" t="s">
         <v>148</v>
       </c>
@@ -3114,6 +3269,10 @@
       <c r="B37" t="s">
         <v>151</v>
       </c>
+      <c r="C37" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>152</v>
       </c>
@@ -3140,6 +3299,10 @@
       <c r="B38" t="s">
         <v>155</v>
       </c>
+      <c r="C38" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D38" s="1" t="s">
         <v>156</v>
       </c>
@@ -3166,6 +3329,10 @@
       <c r="B39" t="s">
         <v>159</v>
       </c>
+      <c r="C39" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Willi@prueba.com</v>
+      </c>
       <c r="D39" s="1" t="s">
         <v>160</v>
       </c>
@@ -3192,6 +3359,10 @@
       <c r="B40" t="s">
         <v>163</v>
       </c>
+      <c r="C40" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>María@prueba.com</v>
+      </c>
       <c r="D40" s="1" t="s">
         <v>164</v>
       </c>
@@ -3218,6 +3389,10 @@
       <c r="B41" t="s">
         <v>167</v>
       </c>
+      <c r="C41" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Emili@prueba.com</v>
+      </c>
       <c r="D41" s="1" t="s">
         <v>168</v>
       </c>
@@ -3244,6 +3419,10 @@
       <c r="B42" t="s">
         <v>171</v>
       </c>
+      <c r="C42" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Santi@prueba.com</v>
+      </c>
       <c r="D42" s="1" t="s">
         <v>172</v>
       </c>
@@ -3270,6 +3449,10 @@
       <c r="B43" t="s">
         <v>175</v>
       </c>
+      <c r="C43" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D43" s="1" t="s">
         <v>176</v>
       </c>
@@ -3296,6 +3479,10 @@
       <c r="B44" t="s">
         <v>179</v>
       </c>
+      <c r="C44" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Adria@prueba.com</v>
+      </c>
       <c r="D44" s="1" t="s">
         <v>180</v>
       </c>
@@ -3322,6 +3509,10 @@
       <c r="B45" t="s">
         <v>183</v>
       </c>
+      <c r="C45" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sofia@prueba.com</v>
+      </c>
       <c r="D45" s="1" t="s">
         <v>184</v>
       </c>
@@ -3348,6 +3539,10 @@
       <c r="B46" t="s">
         <v>187</v>
       </c>
+      <c r="C46" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sofia@prueba.com</v>
+      </c>
       <c r="D46" s="1" t="s">
         <v>188</v>
       </c>
@@ -3374,6 +3569,10 @@
       <c r="B47" t="s">
         <v>191</v>
       </c>
+      <c r="C47" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sandr@prueba.com</v>
+      </c>
       <c r="D47" s="1" t="s">
         <v>192</v>
       </c>
@@ -3400,6 +3599,10 @@
       <c r="B48" t="s">
         <v>195</v>
       </c>
+      <c r="C48" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D48" s="1" t="s">
         <v>196</v>
       </c>
@@ -3426,6 +3629,10 @@
       <c r="B49" t="s">
         <v>199</v>
       </c>
+      <c r="C49" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Carol@prueba.com</v>
+      </c>
       <c r="D49" s="1" t="s">
         <v>200</v>
       </c>
@@ -3452,6 +3659,10 @@
       <c r="B50" t="s">
         <v>203</v>
       </c>
+      <c r="C50" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Samue@prueba.com</v>
+      </c>
       <c r="D50" s="1" t="s">
         <v>204</v>
       </c>
@@ -3478,6 +3689,10 @@
       <c r="B51" t="s">
         <v>207</v>
       </c>
+      <c r="C51" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Natal@prueba.com</v>
+      </c>
       <c r="D51" s="1" t="s">
         <v>208</v>
       </c>
@@ -3504,6 +3719,10 @@
       <c r="B52" t="s">
         <v>211</v>
       </c>
+      <c r="C52" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D52" s="1" t="s">
         <v>212</v>
       </c>
@@ -3533,6 +3752,10 @@
       <c r="B53" t="s">
         <v>216</v>
       </c>
+      <c r="C53" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>André@prueba.com</v>
+      </c>
       <c r="D53" s="1" t="s">
         <v>140</v>
       </c>
@@ -3559,6 +3782,10 @@
       <c r="B54" t="s">
         <v>218</v>
       </c>
+      <c r="C54" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Mateo@prueba.com</v>
+      </c>
       <c r="D54" s="1" t="s">
         <v>219</v>
       </c>
@@ -3585,6 +3812,10 @@
       <c r="B55" t="s">
         <v>222</v>
       </c>
+      <c r="C55" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Lucia@prueba.com</v>
+      </c>
       <c r="D55" s="1" t="s">
         <v>223</v>
       </c>
@@ -3611,6 +3842,10 @@
       <c r="B56" t="s">
         <v>226</v>
       </c>
+      <c r="C56" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D56" s="1" t="s">
         <v>227</v>
       </c>
@@ -3640,6 +3875,10 @@
       <c r="B57" t="s">
         <v>231</v>
       </c>
+      <c r="C57" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Natal@prueba.com</v>
+      </c>
       <c r="D57" s="1" t="s">
         <v>232</v>
       </c>
@@ -3669,6 +3908,10 @@
       <c r="B58" t="s">
         <v>236</v>
       </c>
+      <c r="C58" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D58" s="1" t="s">
         <v>237</v>
       </c>
@@ -3695,6 +3938,10 @@
       <c r="B59" t="s">
         <v>240</v>
       </c>
+      <c r="C59" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D59" s="1" t="s">
         <v>241</v>
       </c>
@@ -3721,6 +3968,10 @@
       <c r="B60" t="s">
         <v>244</v>
       </c>
+      <c r="C60" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Vivia@prueba.com</v>
+      </c>
       <c r="D60" s="1" t="s">
         <v>245</v>
       </c>
@@ -3747,6 +3998,10 @@
       <c r="B61" t="s">
         <v>248</v>
       </c>
+      <c r="C61" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D61" s="1" t="s">
         <v>249</v>
       </c>
@@ -3776,6 +4031,10 @@
       <c r="B62" t="s">
         <v>253</v>
       </c>
+      <c r="C62" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Santi@prueba.com</v>
+      </c>
       <c r="D62" s="1" t="s">
         <v>254</v>
       </c>
@@ -3802,6 +4061,10 @@
       <c r="B63" t="s">
         <v>257</v>
       </c>
+      <c r="C63" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D63" s="1" t="s">
         <v>258</v>
       </c>
@@ -3828,6 +4091,10 @@
       <c r="B64" t="s">
         <v>261</v>
       </c>
+      <c r="C64" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Crist@prueba.com</v>
+      </c>
       <c r="D64" s="1" t="s">
         <v>262</v>
       </c>
@@ -3854,6 +4121,10 @@
       <c r="B65" t="s">
         <v>265</v>
       </c>
+      <c r="C65" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Crist@prueba.com</v>
+      </c>
       <c r="D65" s="1" t="s">
         <v>262</v>
       </c>
@@ -3880,6 +4151,10 @@
       <c r="B66" t="s">
         <v>266</v>
       </c>
+      <c r="C66" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Wendy@prueba.com</v>
+      </c>
       <c r="D66" s="1" t="s">
         <v>267</v>
       </c>
@@ -3906,6 +4181,10 @@
       <c r="B67" t="s">
         <v>270</v>
       </c>
+      <c r="C67" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Janny@prueba.com</v>
+      </c>
       <c r="D67" s="1" t="s">
         <v>271</v>
       </c>
@@ -3932,6 +4211,10 @@
       <c r="B68" t="s">
         <v>274</v>
       </c>
+      <c r="C68" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D68" s="1" t="s">
         <v>275</v>
       </c>
@@ -3958,6 +4241,10 @@
       <c r="B69" t="s">
         <v>278</v>
       </c>
+      <c r="C69" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Julia@prueba.com</v>
+      </c>
       <c r="D69" s="1" t="s">
         <v>279</v>
       </c>
@@ -3984,6 +4271,10 @@
       <c r="B70" t="s">
         <v>282</v>
       </c>
+      <c r="C70" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>CARLO@prueba.com</v>
+      </c>
       <c r="D70" s="1" t="s">
         <v>283</v>
       </c>
@@ -4010,6 +4301,10 @@
       <c r="B71" t="s">
         <v>286</v>
       </c>
+      <c r="C71" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sabri@prueba.com</v>
+      </c>
       <c r="D71" s="1" t="s">
         <v>287</v>
       </c>
@@ -4039,6 +4334,10 @@
       <c r="B72" t="s">
         <v>291</v>
       </c>
+      <c r="C72" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jorge@prueba.com</v>
+      </c>
       <c r="D72" s="1" t="s">
         <v>292</v>
       </c>
@@ -4068,6 +4367,10 @@
       <c r="B73" t="s">
         <v>295</v>
       </c>
+      <c r="C73" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Sofia@prueba.com</v>
+      </c>
       <c r="D73" s="1" t="s">
         <v>296</v>
       </c>
@@ -4094,6 +4397,10 @@
       <c r="B74" t="s">
         <v>299</v>
       </c>
+      <c r="C74" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Ana M@prueba.com</v>
+      </c>
       <c r="D74" s="1" t="s">
         <v>300</v>
       </c>
@@ -4120,6 +4427,10 @@
       <c r="B75" t="s">
         <v>303</v>
       </c>
+      <c r="C75" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Chels@prueba.com</v>
+      </c>
       <c r="D75" s="1" t="s">
         <v>304</v>
       </c>
@@ -4146,6 +4457,10 @@
       <c r="B76" t="s">
         <v>307</v>
       </c>
+      <c r="C76" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>MARIA@prueba.com</v>
+      </c>
       <c r="D76" s="1" t="s">
         <v>308</v>
       </c>
@@ -4172,6 +4487,10 @@
       <c r="B77" t="s">
         <v>311</v>
       </c>
+      <c r="C77" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D77" s="1" t="s">
         <v>312</v>
       </c>
@@ -4198,6 +4517,10 @@
       <c r="B78" t="s">
         <v>315</v>
       </c>
+      <c r="C78" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Alfre@prueba.com</v>
+      </c>
       <c r="D78" s="1" t="s">
         <v>316</v>
       </c>
@@ -4227,6 +4550,10 @@
       <c r="B79" t="s">
         <v>321</v>
       </c>
+      <c r="C79" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Vivia@prueba.com</v>
+      </c>
       <c r="D79" s="1" t="s">
         <v>322</v>
       </c>
@@ -4253,6 +4580,10 @@
       <c r="B80" t="s">
         <v>325</v>
       </c>
+      <c r="C80" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Erika@prueba.com</v>
+      </c>
       <c r="D80" s="1" t="s">
         <v>326</v>
       </c>
@@ -4279,6 +4610,10 @@
       <c r="B81" t="s">
         <v>329</v>
       </c>
+      <c r="C81" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Julia@prueba.com</v>
+      </c>
       <c r="D81" s="1" t="s">
         <v>330</v>
       </c>
@@ -4305,6 +4640,10 @@
       <c r="B82" t="s">
         <v>333</v>
       </c>
+      <c r="C82" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D82" s="1" t="s">
         <v>334</v>
       </c>
@@ -4331,6 +4670,10 @@
       <c r="B83" t="s">
         <v>337</v>
       </c>
+      <c r="C83" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D83" s="1" t="s">
         <v>338</v>
       </c>
@@ -4357,6 +4700,10 @@
       <c r="B84" t="s">
         <v>341</v>
       </c>
+      <c r="C84" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Ana M@prueba.com</v>
+      </c>
       <c r="D84" s="1" t="s">
         <v>342</v>
       </c>
@@ -4383,6 +4730,10 @@
       <c r="B85" t="s">
         <v>345</v>
       </c>
+      <c r="C85" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>David@prueba.com</v>
+      </c>
       <c r="D85" s="1" t="s">
         <v>346</v>
       </c>
@@ -4409,6 +4760,10 @@
       <c r="B86" t="s">
         <v>349</v>
       </c>
+      <c r="C86" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Gabri@prueba.com</v>
+      </c>
       <c r="D86" s="1" t="s">
         <v>350</v>
       </c>
@@ -4435,6 +4790,10 @@
       <c r="B87" t="s">
         <v>353</v>
       </c>
+      <c r="C87" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Natal@prueba.com</v>
+      </c>
       <c r="D87" s="1" t="s">
         <v>354</v>
       </c>
@@ -4461,6 +4820,10 @@
       <c r="B88" t="s">
         <v>357</v>
       </c>
+      <c r="C88" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Miche@prueba.com</v>
+      </c>
       <c r="D88" s="1" t="s">
         <v>358</v>
       </c>
@@ -4490,6 +4853,10 @@
       <c r="B89" t="s">
         <v>362</v>
       </c>
+      <c r="C89" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Paula@prueba.com</v>
+      </c>
       <c r="D89" s="1" t="s">
         <v>363</v>
       </c>
@@ -4516,6 +4883,10 @@
       <c r="B90" t="s">
         <v>366</v>
       </c>
+      <c r="C90" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Santi@prueba.com</v>
+      </c>
       <c r="D90" s="1" t="s">
         <v>367</v>
       </c>
@@ -4542,6 +4913,10 @@
       <c r="B91" t="s">
         <v>370</v>
       </c>
+      <c r="C91" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Giova@prueba.com</v>
+      </c>
       <c r="D91" s="1" t="s">
         <v>371</v>
       </c>
@@ -4568,6 +4943,10 @@
       <c r="B92" t="s">
         <v>374</v>
       </c>
+      <c r="C92" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Melis@prueba.com</v>
+      </c>
       <c r="D92" s="1" t="s">
         <v>375</v>
       </c>
@@ -4594,6 +4973,10 @@
       <c r="B93" t="s">
         <v>378</v>
       </c>
+      <c r="C93" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D93" s="1" t="s">
         <v>379</v>
       </c>
@@ -4623,6 +5006,10 @@
       <c r="B94" t="s">
         <v>383</v>
       </c>
+      <c r="C94" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D94" s="1" t="s">
         <v>384</v>
       </c>
@@ -4649,6 +5036,10 @@
       <c r="B95" t="s">
         <v>387</v>
       </c>
+      <c r="C95" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Manue@prueba.com</v>
+      </c>
       <c r="D95" s="1" t="s">
         <v>388</v>
       </c>
@@ -4678,6 +5069,10 @@
       <c r="B96" t="s">
         <v>392</v>
       </c>
+      <c r="C96" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juliá@prueba.com</v>
+      </c>
       <c r="D96" s="1" t="s">
         <v>393</v>
       </c>
@@ -4704,6 +5099,10 @@
       <c r="B97" t="s">
         <v>396</v>
       </c>
+      <c r="C97" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Aleja@prueba.com</v>
+      </c>
       <c r="D97" s="1" t="s">
         <v>397</v>
       </c>
@@ -4730,6 +5129,10 @@
       <c r="B98" t="s">
         <v>400</v>
       </c>
+      <c r="C98" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D98" s="1" t="s">
         <v>64</v>
       </c>
@@ -4756,6 +5159,10 @@
       <c r="B99" t="s">
         <v>401</v>
       </c>
+      <c r="C99" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D99" s="1" t="s">
         <v>402</v>
       </c>
@@ -4782,6 +5189,10 @@
       <c r="B100" t="s">
         <v>405</v>
       </c>
+      <c r="C100" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D100" s="1" t="s">
         <v>406</v>
       </c>
@@ -4808,6 +5219,10 @@
       <c r="B101" t="s">
         <v>396</v>
       </c>
+      <c r="C101" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Aleja@prueba.com</v>
+      </c>
       <c r="D101" s="1" t="s">
         <v>397</v>
       </c>
@@ -4834,6 +5249,10 @@
       <c r="B102" t="s">
         <v>409</v>
       </c>
+      <c r="C102" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>André@prueba.com</v>
+      </c>
       <c r="D102" s="1" t="s">
         <v>410</v>
       </c>
@@ -4860,6 +5279,10 @@
       <c r="B103" t="s">
         <v>413</v>
       </c>
+      <c r="C103" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Catal@prueba.com</v>
+      </c>
       <c r="D103" s="1" t="s">
         <v>414</v>
       </c>
@@ -4886,6 +5309,10 @@
       <c r="B104" t="s">
         <v>417</v>
       </c>
+      <c r="C104" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Angel@prueba.com</v>
+      </c>
       <c r="D104" s="1" t="s">
         <v>418</v>
       </c>
@@ -4912,6 +5339,10 @@
       <c r="B105" t="s">
         <v>79</v>
       </c>
+      <c r="C105" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Ximen@prueba.com</v>
+      </c>
       <c r="D105" s="1" t="s">
         <v>80</v>
       </c>
@@ -4938,6 +5369,10 @@
       <c r="B106" t="s">
         <v>421</v>
       </c>
+      <c r="C106" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>César@prueba.com</v>
+      </c>
       <c r="D106" s="1" t="s">
         <v>422</v>
       </c>
@@ -4964,6 +5399,10 @@
       <c r="B107" t="s">
         <v>425</v>
       </c>
+      <c r="C107" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>juan @prueba.com</v>
+      </c>
       <c r="D107" s="1" t="s">
         <v>426</v>
       </c>
@@ -4990,6 +5429,10 @@
       <c r="B108" t="s">
         <v>428</v>
       </c>
+      <c r="C108" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D108" s="1" t="s">
         <v>429</v>
       </c>
@@ -5016,6 +5459,10 @@
       <c r="B109" t="s">
         <v>432</v>
       </c>
+      <c r="C109" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nesto@prueba.com</v>
+      </c>
       <c r="D109" s="1" t="s">
         <v>433</v>
       </c>
@@ -5042,6 +5489,10 @@
       <c r="B110" t="s">
         <v>436</v>
       </c>
+      <c r="C110" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Saulo@prueba.com</v>
+      </c>
       <c r="D110" s="1" t="s">
         <v>437</v>
       </c>
@@ -5071,6 +5522,10 @@
       <c r="B111" t="s">
         <v>103</v>
       </c>
+      <c r="C111" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D111" s="1" t="s">
         <v>441</v>
       </c>
@@ -5097,6 +5552,10 @@
       <c r="B112" t="s">
         <v>442</v>
       </c>
+      <c r="C112" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D112" s="1" t="s">
         <v>443</v>
       </c>
@@ -5123,6 +5582,10 @@
       <c r="B113" t="s">
         <v>442</v>
       </c>
+      <c r="C113" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D113" s="1" t="s">
         <v>446</v>
       </c>
@@ -5149,6 +5612,10 @@
       <c r="B114" t="s">
         <v>447</v>
       </c>
+      <c r="C114" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D114" s="1" t="s">
         <v>448</v>
       </c>
@@ -5175,6 +5642,10 @@
       <c r="B115" t="s">
         <v>67</v>
       </c>
+      <c r="C115" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Andre@prueba.com</v>
+      </c>
       <c r="D115" s="1" t="s">
         <v>68</v>
       </c>
@@ -5201,6 +5672,10 @@
       <c r="B116" t="s">
         <v>452</v>
       </c>
+      <c r="C116" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D116" s="1" t="s">
         <v>453</v>
       </c>
@@ -5227,6 +5702,10 @@
       <c r="B117" t="s">
         <v>456</v>
       </c>
+      <c r="C117" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D117" s="1" t="s">
         <v>457</v>
       </c>
@@ -5256,6 +5735,10 @@
       <c r="B118" t="s">
         <v>461</v>
       </c>
+      <c r="C118" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D118" s="1" t="s">
         <v>462</v>
       </c>
@@ -5282,6 +5765,10 @@
       <c r="B119" t="s">
         <v>465</v>
       </c>
+      <c r="C119" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D119" s="1" t="s">
         <v>466</v>
       </c>
@@ -5308,6 +5795,10 @@
       <c r="B120" t="s">
         <v>469</v>
       </c>
+      <c r="C120" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Santi@prueba.com</v>
+      </c>
       <c r="D120" s="1" t="s">
         <v>470</v>
       </c>
@@ -5334,6 +5825,10 @@
       <c r="B121" t="s">
         <v>473</v>
       </c>
+      <c r="C121" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D121" s="1" t="s">
         <v>474</v>
       </c>
@@ -5360,6 +5855,10 @@
       <c r="B122" t="s">
         <v>477</v>
       </c>
+      <c r="C122" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Valen@prueba.com</v>
+      </c>
       <c r="D122" s="1" t="s">
         <v>478</v>
       </c>
@@ -5389,6 +5888,10 @@
       <c r="B123" t="s">
         <v>482</v>
       </c>
+      <c r="C123" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Franc@prueba.com</v>
+      </c>
       <c r="D123" s="1" t="s">
         <v>483</v>
       </c>
@@ -5415,6 +5918,10 @@
       <c r="B124" t="s">
         <v>486</v>
       </c>
+      <c r="C124" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Martí@prueba.com</v>
+      </c>
       <c r="D124" s="1" t="s">
         <v>487</v>
       </c>
@@ -5441,6 +5948,10 @@
       <c r="B125" t="s">
         <v>490</v>
       </c>
+      <c r="C125" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D125" s="1" t="s">
         <v>491</v>
       </c>
@@ -5467,6 +5978,10 @@
       <c r="B126" t="s">
         <v>494</v>
       </c>
+      <c r="C126" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>David@prueba.com</v>
+      </c>
       <c r="D126" s="1" t="s">
         <v>495</v>
       </c>
@@ -5493,6 +6008,10 @@
       <c r="B127" t="s">
         <v>473</v>
       </c>
+      <c r="C127" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Danie@prueba.com</v>
+      </c>
       <c r="D127" s="1" t="s">
         <v>498</v>
       </c>
@@ -5519,6 +6038,10 @@
       <c r="B128" t="s">
         <v>499</v>
       </c>
+      <c r="C128" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Bryan@prueba.com</v>
+      </c>
       <c r="D128" s="1" t="s">
         <v>500</v>
       </c>
@@ -5545,6 +6068,10 @@
       <c r="B129" t="s">
         <v>503</v>
       </c>
+      <c r="C129" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Carlo@prueba.com</v>
+      </c>
       <c r="D129" s="1" t="s">
         <v>504</v>
       </c>
@@ -5571,6 +6098,10 @@
       <c r="B130" t="s">
         <v>211</v>
       </c>
+      <c r="C130" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D130" s="1" t="s">
         <v>212</v>
       </c>
@@ -5600,6 +6131,10 @@
       <c r="B131" t="s">
         <v>508</v>
       </c>
+      <c r="C131" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D131" s="1" t="s">
         <v>441</v>
       </c>
@@ -5626,6 +6161,10 @@
       <c r="B132" t="s">
         <v>509</v>
       </c>
+      <c r="C132" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Willi@prueba.com</v>
+      </c>
       <c r="D132" s="1" t="s">
         <v>160</v>
       </c>
@@ -5652,6 +6191,10 @@
       <c r="B133" t="s">
         <v>511</v>
       </c>
+      <c r="C133" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Maria@prueba.com</v>
+      </c>
       <c r="D133" s="1" t="s">
         <v>108</v>
       </c>
@@ -5678,6 +6221,10 @@
       <c r="B134" t="s">
         <v>512</v>
       </c>
+      <c r="C134" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D134" s="1" t="s">
         <v>448</v>
       </c>
@@ -5704,6 +6251,10 @@
       <c r="B135" t="s">
         <v>513</v>
       </c>
+      <c r="C135" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Chels@prueba.com</v>
+      </c>
       <c r="D135" s="1" t="s">
         <v>304</v>
       </c>
@@ -5730,6 +6281,10 @@
       <c r="B136" t="s">
         <v>111</v>
       </c>
+      <c r="C136" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Tábat@prueba.com</v>
+      </c>
       <c r="D136" s="1" t="s">
         <v>112</v>
       </c>
@@ -5756,6 +6311,10 @@
       <c r="B137" t="s">
         <v>514</v>
       </c>
+      <c r="C137" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D137" s="1" t="s">
         <v>176</v>
       </c>
@@ -5782,6 +6341,10 @@
       <c r="B138" t="s">
         <v>515</v>
       </c>
+      <c r="C138" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jorge@prueba.com</v>
+      </c>
       <c r="D138" s="1" t="s">
         <v>116</v>
       </c>
@@ -5808,6 +6371,10 @@
       <c r="B139" t="s">
         <v>353</v>
       </c>
+      <c r="C139" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Natal@prueba.com</v>
+      </c>
       <c r="D139" s="1" t="s">
         <v>354</v>
       </c>
@@ -5834,6 +6401,10 @@
       <c r="B140" t="s">
         <v>516</v>
       </c>
+      <c r="C140" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D140" s="1" t="s">
         <v>517</v>
       </c>
@@ -5860,6 +6431,10 @@
       <c r="B141" t="s">
         <v>520</v>
       </c>
+      <c r="C141" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Aleja@prueba.com</v>
+      </c>
       <c r="D141" s="1" t="s">
         <v>521</v>
       </c>
@@ -5886,6 +6461,10 @@
       <c r="B142" t="s">
         <v>524</v>
       </c>
+      <c r="C142" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Juan @prueba.com</v>
+      </c>
       <c r="D142" s="1" t="s">
         <v>338</v>
       </c>
@@ -5912,6 +6491,10 @@
       <c r="B143" t="s">
         <v>525</v>
       </c>
+      <c r="C143" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D143" s="1" t="s">
         <v>241</v>
       </c>
@@ -5938,6 +6521,10 @@
       <c r="B144" t="s">
         <v>526</v>
       </c>
+      <c r="C144" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Felip@prueba.com</v>
+      </c>
       <c r="D144" s="1" t="s">
         <v>527</v>
       </c>
@@ -5964,6 +6551,10 @@
       <c r="B145" t="s">
         <v>530</v>
       </c>
+      <c r="C145" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jorge@prueba.com</v>
+      </c>
       <c r="D145" s="1" t="s">
         <v>531</v>
       </c>
@@ -5990,6 +6581,10 @@
       <c r="B146" t="s">
         <v>534</v>
       </c>
+      <c r="C146" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D146" s="1" t="s">
         <v>535</v>
       </c>
@@ -6016,6 +6611,10 @@
       <c r="B147" t="s">
         <v>538</v>
       </c>
+      <c r="C147" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Andre@prueba.com</v>
+      </c>
       <c r="D147" s="1" t="s">
         <v>539</v>
       </c>
@@ -6042,6 +6641,10 @@
       <c r="B148" t="s">
         <v>542</v>
       </c>
+      <c r="C148" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Simón@prueba.com</v>
+      </c>
       <c r="D148" s="1" t="s">
         <v>543</v>
       </c>
@@ -6071,6 +6674,10 @@
       <c r="B149" t="s">
         <v>547</v>
       </c>
+      <c r="C149" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jonat@prueba.com</v>
+      </c>
       <c r="D149" s="1" t="s">
         <v>548</v>
       </c>
@@ -6097,6 +6704,10 @@
       <c r="B150" t="s">
         <v>551</v>
       </c>
+      <c r="C150" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Mateo@prueba.com</v>
+      </c>
       <c r="D150" s="1" t="s">
         <v>552</v>
       </c>
@@ -6123,6 +6734,10 @@
       <c r="B151" t="s">
         <v>442</v>
       </c>
+      <c r="C151" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Nicol@prueba.com</v>
+      </c>
       <c r="D151" s="1" t="s">
         <v>446</v>
       </c>
@@ -6149,6 +6764,10 @@
       <c r="B152" t="s">
         <v>555</v>
       </c>
+      <c r="C152" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Migue@prueba.com</v>
+      </c>
       <c r="D152" s="1" t="s">
         <v>556</v>
       </c>
@@ -6178,6 +6797,10 @@
       <c r="B153" t="s">
         <v>560</v>
       </c>
+      <c r="C153" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Gabri@prueba.com</v>
+      </c>
       <c r="D153" s="1" t="s">
         <v>561</v>
       </c>
@@ -6204,6 +6827,10 @@
       <c r="B154" t="s">
         <v>560</v>
       </c>
+      <c r="C154" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Gabri@prueba.com</v>
+      </c>
       <c r="D154" s="1" t="s">
         <v>561</v>
       </c>
@@ -6233,6 +6860,10 @@
       <c r="B155" t="s">
         <v>530</v>
       </c>
+      <c r="C155" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Jorge@prueba.com</v>
+      </c>
       <c r="D155" s="1" t="s">
         <v>531</v>
       </c>
@@ -6259,6 +6890,10 @@
       <c r="B156" t="s">
         <v>565</v>
       </c>
+      <c r="C156" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Laura@prueba.com</v>
+      </c>
       <c r="D156" s="1" t="s">
         <v>535</v>
       </c>
@@ -6285,6 +6920,10 @@
       <c r="B157" t="s">
         <v>566</v>
       </c>
+      <c r="C157" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>Gabri@prueba.com</v>
+      </c>
       <c r="D157" s="1" t="s">
         <v>561</v>
       </c>
@@ -6310,6 +6949,10 @@
       </c>
       <c r="B158" t="s">
         <v>409</v>
+      </c>
+      <c r="C158" t="str">
+        <f>_xlfn.CONCAT(LEFT(Table1[[#This Row],[Nombre completo ]],5),"@prueba.com")</f>
+        <v>André@prueba.com</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>410</v>

</xml_diff>